<commit_message>
Included column names, fixed unknown problem, added function so that dataframes of different sizes can be compared
</commit_message>
<xml_diff>
--- a/use_tools/excel_table_comparison/excel_files/changed_groceries.xlsx
+++ b/use_tools/excel_table_comparison/excel_files/changed_groceries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daisyxiao/Desktop/table-processing/use_tools/excel_table_comparison/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED523FF-5961-5341-9093-E5B1AF57DA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D407709A-B390-D840-9C7E-ADB173760A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10500" yWindow="500" windowWidth="16680" windowHeight="15700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -815,15 +815,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F4C8D47-9A72-6C47-AE5A-22C8E3BC943D}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -832,7 +832,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="2">
         <v>3.76</v>
       </c>
@@ -843,7 +843,7 @@
         <v>3.76</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="2">
         <v>6.98</v>
       </c>
@@ -854,7 +854,7 @@
         <v>6.98</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="2">
         <v>7.96</v>
       </c>
@@ -865,7 +865,7 @@
         <v>7.96</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="2">
         <v>3.98</v>
       </c>
@@ -876,7 +876,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="2">
         <v>8.98</v>
       </c>
@@ -887,7 +887,7 @@
         <v>8.98</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="2">
         <v>5.76</v>
       </c>
@@ -898,7 +898,7 @@
         <v>5.76</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="2">
         <v>2.66</v>
       </c>
@@ -909,7 +909,7 @@
         <v>2.66</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="2">
         <v>7.98</v>
       </c>
@@ -920,7 +920,7 @@
         <v>7.98</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>9.6300000000000008</v>
       </c>
@@ -931,7 +931,7 @@
         <v>9.6300000000000008</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="2">
         <v>5.98</v>
       </c>
@@ -942,7 +942,7 @@
         <v>5.98</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12" s="2">
         <v>3.98</v>
       </c>
@@ -952,8 +952,11 @@
       <c r="C12" s="2">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="K12">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="2">
         <v>3.96</v>
       </c>
@@ -964,7 +967,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14" s="2">
         <v>5.98</v>
       </c>
@@ -975,7 +978,7 @@
         <v>5.98</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
         <v>5.98</v>
       </c>
@@ -986,7 +989,7 @@
         <v>5.98</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16" s="2">
         <v>4.28</v>
       </c>

</xml_diff>

<commit_message>
Put stats on summary sheet and remove from individual sheets
</commit_message>
<xml_diff>
--- a/use_tools/excel_table_comparison/excel_files/changed_groceries.xlsx
+++ b/use_tools/excel_table_comparison/excel_files/changed_groceries.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daisyxiao/Desktop/table-processing/use_tools/excel_table_comparison/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D407709A-B390-D840-9C7E-ADB173760A5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB2122D-39B6-7F46-A65A-CD5F53554E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10500" yWindow="500" windowWidth="16680" windowHeight="15700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10500" yWindow="500" windowWidth="16680" windowHeight="15700" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grocery List" sheetId="1" r:id="rId1"/>
     <sheet name="Table 1" sheetId="2" r:id="rId2"/>
     <sheet name="Table 7" sheetId="3" r:id="rId3"/>
+    <sheet name="Random" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="25">
   <si>
     <t>Sardines (copy)</t>
   </si>
@@ -107,6 +108,9 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -817,7 +821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F4C8D47-9A72-6C47-AE5A-22C8E3BC943D}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -1036,4 +1040,1171 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{490BBEBD-1DD2-6B47-8306-B449A1361341}">
+  <dimension ref="A1:J36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A36" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>